<commit_message>
Updating alpha data, completing protons
</commit_message>
<xml_diff>
--- a/Simulations/SRIM_AlphasVsFilters/DataAnalysis/ThickFilter_Analysis.xlsx
+++ b/Simulations/SRIM_AlphasVsFilters/DataAnalysis/ThickFilter_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\Documents\GitHub\xmm-newton\Simulations\SRIM_AlphasVsFilters\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B7CA38-D39F-45D1-ADA3-9F7BED5E3D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0052F56C-60B8-4C1C-926D-C0E98E262DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A9EDBC4B-5209-4052-BD5C-CBCCBA64D68C}"/>
   </bookViews>
@@ -313,10 +313,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Foglio1!$E$6:$E$21</c:f>
+                <c:f>Foglio1!$E$6:$E$23</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="16"/>
+                  <c:ptCount val="18"/>
                   <c:pt idx="0">
                     <c:v>0</c:v>
                   </c:pt>
@@ -333,47 +333,53 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.7004852641</c:v>
+                    <c:v>0.7</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.464022183</c:v>
+                    <c:v>1.464</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>2.3520732744999999</c:v>
+                    <c:v>2.3519999999999999</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>2.7026149650000004</c:v>
+                    <c:v>2.7029999999999998</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>2.9743950982</c:v>
+                    <c:v>2.9740000000000002</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>3.1868145032999999</c:v>
+                    <c:v>3.1869999999999998</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>3.4288823130999999</c:v>
+                    <c:v>3.4289999999999998</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>3.7651729402999998</c:v>
+                    <c:v>3.7650000000000001</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>3.6488864213999999</c:v>
+                    <c:v>3.649</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>3.583304982</c:v>
+                    <c:v>3.5830000000000002</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>2.9789431156999999</c:v>
+                    <c:v>2.9790000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.8969999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>5.0119999999999996</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Foglio1!$E$6:$E$21</c:f>
+                <c:f>Foglio1!$E$6:$E$23</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="16"/>
+                  <c:ptCount val="18"/>
                   <c:pt idx="0">
                     <c:v>0</c:v>
                   </c:pt>
@@ -390,37 +396,43 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.7004852641</c:v>
+                    <c:v>0.7</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.464022183</c:v>
+                    <c:v>1.464</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>2.3520732744999999</c:v>
+                    <c:v>2.3519999999999999</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>2.7026149650000004</c:v>
+                    <c:v>2.7029999999999998</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>2.9743950982</c:v>
+                    <c:v>2.9740000000000002</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>3.1868145032999999</c:v>
+                    <c:v>3.1869999999999998</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>3.4288823130999999</c:v>
+                    <c:v>3.4289999999999998</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>3.7651729402999998</c:v>
+                    <c:v>3.7650000000000001</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>3.6488864213999999</c:v>
+                    <c:v>3.649</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>3.583304982</c:v>
+                    <c:v>3.5830000000000002</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>2.9789431156999999</c:v>
+                    <c:v>2.9790000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.8969999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>5.0119999999999996</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -441,10 +453,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Foglio1!$A$6:$A$21</c:f>
+              <c:f>Foglio1!$A$6:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -492,16 +504,22 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Foglio1!$C$6:$C$21</c:f>
+              <c:f>Foglio1!$C$6:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -549,6 +567,12 @@
                 </c:pt>
                 <c:pt idx="15" formatCode="0.0">
                   <c:v>82.219899999999996</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.0">
+                  <c:v>99.901200000000003</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.0">
+                  <c:v>118.018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,10 +998,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Foglio1!$H$6:$H$21</c:f>
+                <c:f>Foglio1!$H$6:$H$23</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="16"/>
+                  <c:ptCount val="18"/>
                   <c:pt idx="0">
                     <c:v>0</c:v>
                   </c:pt>
@@ -994,47 +1018,53 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>29.647324391404489</c:v>
+                    <c:v>29.62678608328363</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>26.077343364736013</c:v>
+                    <c:v>26.076948238408981</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>17.102593174914691</c:v>
+                    <c:v>17.102060375202548</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>18.120368046017802</c:v>
+                    <c:v>18.122949610909927</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>11.925061612956132</c:v>
+                    <c:v>11.923477569739742</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>12.698015041610775</c:v>
+                    <c:v>12.698754162097497</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>9.779531889995809</c:v>
+                    <c:v>9.7798675453745858</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>8.4946986205232413</c:v>
+                    <c:v>8.4943084456890077</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>6.8928197873569799</c:v>
+                    <c:v>6.8930343396151468</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>5.8375062184837514</c:v>
+                    <c:v>5.8370093770676652</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>4.2673393918194691</c:v>
+                    <c:v>4.2674208786437351</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>4.8799215985393563</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>5.6050245216831325</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Foglio1!$H$6:$H$21</c:f>
+                <c:f>Foglio1!$H$6:$H$23</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="16"/>
+                  <c:ptCount val="18"/>
                   <c:pt idx="0">
                     <c:v>0</c:v>
                   </c:pt>
@@ -1051,37 +1081,43 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>29.647324391404489</c:v>
+                    <c:v>29.62678608328363</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>26.077343364736013</c:v>
+                    <c:v>26.076948238408981</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>17.102593174914691</c:v>
+                    <c:v>17.102060375202548</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>18.120368046017802</c:v>
+                    <c:v>18.122949610909927</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>11.925061612956132</c:v>
+                    <c:v>11.923477569739742</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>12.698015041610775</c:v>
+                    <c:v>12.698754162097497</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>9.779531889995809</c:v>
+                    <c:v>9.7798675453745858</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>8.4946986205232413</c:v>
+                    <c:v>8.4943084456890077</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>6.8928197873569799</c:v>
+                    <c:v>6.8930343396151468</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>5.8375062184837514</c:v>
+                    <c:v>5.8370093770676652</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>4.2673393918194691</c:v>
+                    <c:v>4.2674208786437351</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>4.8799215985393563</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>5.6050245216831325</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1102,10 +1138,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Foglio1!$A$6:$A$21</c:f>
+              <c:f>Foglio1!$A$6:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1153,16 +1189,22 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Foglio1!$G$6:$G$21</c:f>
+              <c:f>Foglio1!$G$6:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0" formatCode="0.00">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1210,6 +1252,12 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>117.7801</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>125.0988</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>131.982</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1629,108 +1677,96 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Foglio1!$E$7:$E$21</c:f>
+                <c:f>Foglio1!$E$11:$E$23</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="15"/>
+                  <c:ptCount val="13"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.7</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>1.464</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>2.3519999999999999</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>2.7029999999999998</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.7004852641</c:v>
+                    <c:v>2.9740000000000002</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.464022183</c:v>
+                    <c:v>3.1869999999999998</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>2.3520732744999999</c:v>
+                    <c:v>3.4289999999999998</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>2.7026149650000004</c:v>
+                    <c:v>3.7650000000000001</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>2.9743950982</c:v>
+                    <c:v>3.649</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>3.1868145032999999</c:v>
+                    <c:v>3.5830000000000002</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>3.4288823130999999</c:v>
+                    <c:v>2.9790000000000001</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>3.7651729402999998</c:v>
+                    <c:v>3.8969999999999998</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>3.6488864213999999</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>3.583304982</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>2.9789431156999999</c:v>
+                    <c:v>5.0119999999999996</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Foglio1!$E$7:$E$21</c:f>
+                <c:f>Foglio1!$E$11:$E$23</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="15"/>
+                  <c:ptCount val="13"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.7</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>1.464</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>2.3519999999999999</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>2.7029999999999998</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.7004852641</c:v>
+                    <c:v>2.9740000000000002</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.464022183</c:v>
+                    <c:v>3.1869999999999998</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>2.3520732744999999</c:v>
+                    <c:v>3.4289999999999998</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>2.7026149650000004</c:v>
+                    <c:v>3.7650000000000001</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>2.9743950982</c:v>
+                    <c:v>3.649</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>3.1868145032999999</c:v>
+                    <c:v>3.5830000000000002</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>3.4288823130999999</c:v>
+                    <c:v>2.9790000000000001</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>3.7651729402999998</c:v>
+                    <c:v>3.8969999999999998</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>3.6488864213999999</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>3.583304982</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>2.9789431156999999</c:v>
+                    <c:v>5.0119999999999996</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1756,108 +1792,96 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Foglio1!$H$7:$H$21</c:f>
+                <c:f>Foglio1!$H$11:$H$23</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="15"/>
+                  <c:ptCount val="13"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>29.62678608328363</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>26.076948238408981</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>17.102060375202548</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>18.122949610909927</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>29.647324391404489</c:v>
+                    <c:v>11.923477569739742</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>26.077343364736013</c:v>
+                    <c:v>12.698754162097497</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>17.102593174914691</c:v>
+                    <c:v>9.7798675453745858</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>18.120368046017802</c:v>
+                    <c:v>8.4943084456890077</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>11.925061612956132</c:v>
+                    <c:v>6.8930343396151468</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>12.698015041610775</c:v>
+                    <c:v>5.8370093770676652</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>9.779531889995809</c:v>
+                    <c:v>4.2674208786437351</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>8.4946986205232413</c:v>
+                    <c:v>4.8799215985393563</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>6.8928197873569799</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>5.8375062184837514</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>4.2673393918194691</c:v>
+                    <c:v>5.6050245216831325</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Foglio1!$H$7:$H$21</c:f>
+                <c:f>Foglio1!$H$11:$H$23</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="15"/>
+                  <c:ptCount val="13"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>29.62678608328363</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>26.076948238408981</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>17.102060375202548</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>18.122949610909927</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>29.647324391404489</c:v>
+                    <c:v>11.923477569739742</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>26.077343364736013</c:v>
+                    <c:v>12.698754162097497</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>17.102593174914691</c:v>
+                    <c:v>9.7798675453745858</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>18.120368046017802</c:v>
+                    <c:v>8.4943084456890077</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>11.925061612956132</c:v>
+                    <c:v>6.8930343396151468</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>12.698015041610775</c:v>
+                    <c:v>5.8370093770676652</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>9.779531889995809</c:v>
+                    <c:v>4.2674208786437351</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>8.4946986205232413</c:v>
+                    <c:v>4.8799215985393563</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>6.8928197873569799</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>5.8375062184837514</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>4.2673393918194691</c:v>
+                    <c:v>5.6050245216831325</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1878,108 +1902,96 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Foglio1!$C$7:$C$21</c:f>
+              <c:f>Foglio1!$C$11:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0" formatCode="0.00">
-                  <c:v>0</c:v>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.1540952577000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.1894326673000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>8.4630147549999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>10.3832</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1540952577000001</c:v>
+                  <c:v>17.966799999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1894326673000002</c:v>
+                  <c:v>20.062000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.4630147549999997</c:v>
+                  <c:v>31.151799999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.3832</c:v>
+                  <c:v>42.995899999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.966799999999999</c:v>
+                  <c:v>55.382100000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.062000000000001</c:v>
+                  <c:v>68.4649</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31.151799999999998</c:v>
+                  <c:v>82.219899999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42.995899999999999</c:v>
+                  <c:v>99.901200000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>55.382100000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>68.4649</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>82.219899999999996</c:v>
+                  <c:v>118.018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Foglio1!$G$7:$G$21</c:f>
+              <c:f>Foglio1!$G$11:$G$23</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:formatCode>#,#00</c:formatCode>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>48.8459047423</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>56.810567332700003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>61.536985244999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>69.616799999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.8459047423</c:v>
+                  <c:v>72.033199999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.810567332700003</c:v>
+                  <c:v>79.938000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>61.536985244999997</c:v>
+                  <c:v>88.848200000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>69.616799999999998</c:v>
+                  <c:v>97.004099999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.033199999999994</c:v>
+                  <c:v>104.61789999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>79.938000000000002</c:v>
+                  <c:v>111.5351</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.848200000000006</c:v>
+                  <c:v>117.7801</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>97.004099999999994</c:v>
+                  <c:v>125.0988</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.61789999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>111.5351</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>117.7801</c:v>
+                  <c:v>131.982</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1987,11 +1999,12 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-27A8-4D32-A8E2-B84A489EEB9C}"/>
+              <c16:uniqueId val="{00000000-0F0C-4902-B74F-F77732F067A1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2079,7 +2092,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2196,7 +2209,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3956,15 +3969,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>3554</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>4583</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3992,15 +4005,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>402</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>4296</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4034,7 +4047,7 @@
       <xdr:rowOff>144</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -4621,7 +4634,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="7">
-        <v>0.32319999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -4637,16 +4650,15 @@
         <v>1.1540952577000001</v>
       </c>
       <c r="D11" s="6">
-        <f>7004852641/10000000</f>
-        <v>700.48526409999999</v>
+        <v>700</v>
       </c>
       <c r="E11" s="8">
         <f t="shared" si="1"/>
-        <v>0.7004852641</v>
+        <v>0.7</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" ref="F8:F21" si="4">E11/C11</f>
-        <v>0.60695619311008975</v>
+        <f t="shared" ref="F11:F21" si="4">E11/C11</f>
+        <v>0.6065357216656726</v>
       </c>
       <c r="G11" s="8">
         <f t="shared" si="2"/>
@@ -4654,7 +4666,7 @@
       </c>
       <c r="H11" s="8">
         <f t="shared" si="3"/>
-        <v>29.647324391404489</v>
+        <v>29.62678608328363</v>
       </c>
       <c r="I11" s="7">
         <v>4.3099999999999999E-2</v>
@@ -4673,16 +4685,15 @@
         <v>3.1894326673000002</v>
       </c>
       <c r="D12" s="6">
-        <f>14640221830/10000000</f>
-        <v>1464.022183</v>
+        <v>1464</v>
       </c>
       <c r="E12" s="8">
         <f t="shared" si="1"/>
-        <v>1.464022183</v>
+        <v>1.464</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="4"/>
-        <v>0.45902275912893353</v>
+        <v>0.45901580397348302</v>
       </c>
       <c r="G12" s="8">
         <f t="shared" si="2"/>
@@ -4690,7 +4701,7 @@
       </c>
       <c r="H12" s="8">
         <f t="shared" si="3"/>
-        <v>26.077343364736013</v>
+        <v>26.076948238408981</v>
       </c>
       <c r="I12" s="7">
         <v>0.32319999999999999</v>
@@ -4709,16 +4720,15 @@
         <v>8.4630147549999997</v>
       </c>
       <c r="D13" s="6">
-        <f>23520732745/10000000</f>
-        <v>2352.0732745</v>
+        <v>2352</v>
       </c>
       <c r="E13" s="8">
         <f t="shared" si="1"/>
-        <v>2.3520732744999999</v>
+        <v>2.3519999999999999</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="4"/>
-        <v>0.27792380642020986</v>
+        <v>0.27791514821717928</v>
       </c>
       <c r="G13" s="8">
         <f t="shared" si="2"/>
@@ -4726,7 +4736,7 @@
       </c>
       <c r="H13" s="8">
         <f t="shared" si="3"/>
-        <v>17.102593174914691</v>
+        <v>17.102060375202548</v>
       </c>
       <c r="I13" s="7">
         <v>0.81379999999999997</v>
@@ -4745,16 +4755,15 @@
         <v>10.3832</v>
       </c>
       <c r="D14" s="6">
-        <f>27026149650/10000000</f>
-        <v>2702.6149650000002</v>
+        <v>2703</v>
       </c>
       <c r="E14" s="8">
         <f t="shared" si="1"/>
-        <v>2.7026149650000004</v>
+        <v>2.7029999999999998</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="4"/>
-        <v>0.26028728763772252</v>
+        <v>0.26032437013637411</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" si="2"/>
@@ -4762,7 +4771,7 @@
       </c>
       <c r="H14" s="8">
         <f t="shared" si="3"/>
-        <v>18.120368046017802</v>
+        <v>18.122949610909927</v>
       </c>
       <c r="I14" s="7">
         <v>0.79059999999999997</v>
@@ -4781,16 +4790,15 @@
         <v>17.966799999999999</v>
       </c>
       <c r="D15" s="6">
-        <f>29743950982/10000000</f>
-        <v>2974.3950982000001</v>
+        <v>2974</v>
       </c>
       <c r="E15" s="8">
         <f t="shared" si="1"/>
-        <v>2.9743950982</v>
+        <v>2.9740000000000002</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="4"/>
-        <v>0.16554951901284592</v>
+        <v>0.16552752855266381</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="2"/>
@@ -4798,7 +4806,7 @@
       </c>
       <c r="H15" s="8">
         <f t="shared" si="3"/>
-        <v>11.925061612956132</v>
+        <v>11.923477569739742</v>
       </c>
       <c r="I15" s="7">
         <v>0.94889999999999997</v>
@@ -4817,16 +4825,15 @@
         <v>20.062000000000001</v>
       </c>
       <c r="D16" s="6">
-        <f>31868145033/10000000</f>
-        <v>3186.8145033000001</v>
+        <v>3187</v>
       </c>
       <c r="E16" s="8">
         <f t="shared" si="1"/>
-        <v>3.1868145032999999</v>
+        <v>3.1869999999999998</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="4"/>
-        <v>0.15884829544910775</v>
+        <v>0.15885754162097496</v>
       </c>
       <c r="G16" s="8">
         <f t="shared" si="2"/>
@@ -4834,7 +4841,7 @@
       </c>
       <c r="H16" s="8">
         <f t="shared" si="3"/>
-        <v>12.698015041610775</v>
+        <v>12.698754162097497</v>
       </c>
       <c r="I16" s="7">
         <v>0.93489999999999995</v>
@@ -4854,16 +4861,15 @@
         <v>31.151799999999998</v>
       </c>
       <c r="D17" s="6">
-        <f>34288823131/10000000</f>
-        <v>3428.8823130999999</v>
+        <v>3429</v>
       </c>
       <c r="E17" s="8">
         <f t="shared" si="1"/>
-        <v>3.4288823130999999</v>
+        <v>3.4289999999999998</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="4"/>
-        <v>0.11007011835913175</v>
+        <v>0.11007389621145487</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="2"/>
@@ -4871,7 +4877,7 @@
       </c>
       <c r="H17" s="8">
         <f t="shared" si="3"/>
-        <v>9.779531889995809</v>
+        <v>9.7798675453745858</v>
       </c>
       <c r="I17" s="7">
         <v>0.99</v>
@@ -4891,16 +4897,15 @@
         <v>42.995899999999999</v>
       </c>
       <c r="D18" s="6">
-        <f>37651729403/10000000</f>
-        <v>3765.1729402999999</v>
+        <v>3765</v>
       </c>
       <c r="E18" s="8">
         <f t="shared" si="1"/>
-        <v>3.7651729402999998</v>
+        <v>3.7650000000000001</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="4"/>
-        <v>8.7570511148737443E-2</v>
+        <v>8.7566488897778627E-2</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" si="2"/>
@@ -4908,7 +4913,7 @@
       </c>
       <c r="H18" s="8">
         <f t="shared" si="3"/>
-        <v>8.4946986205232413</v>
+        <v>8.4943084456890077</v>
       </c>
       <c r="I18" s="7">
         <v>0.99</v>
@@ -4928,16 +4933,15 @@
         <v>55.382100000000001</v>
       </c>
       <c r="D19" s="6">
-        <f>36488864214/10000000</f>
-        <v>3648.8864214</v>
+        <v>3649</v>
       </c>
       <c r="E19" s="8">
         <f t="shared" si="1"/>
-        <v>3.6488864213999999</v>
+        <v>3.649</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="4"/>
-        <v>6.5885663804731126E-2</v>
+        <v>6.588771462259467E-2</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" si="2"/>
@@ -4945,7 +4949,7 @@
       </c>
       <c r="H19" s="8">
         <f t="shared" si="3"/>
-        <v>6.8928197873569799</v>
+        <v>6.8930343396151468</v>
       </c>
       <c r="I19" s="7">
         <v>0.99099999999999999</v>
@@ -4965,16 +4969,15 @@
         <v>68.4649</v>
       </c>
       <c r="D20" s="6">
-        <f>35833049820/10000000</f>
-        <v>3583.3049820000001</v>
+        <v>3583</v>
       </c>
       <c r="E20" s="8">
         <f t="shared" si="1"/>
-        <v>3.583304982</v>
+        <v>3.5830000000000002</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="4"/>
-        <v>5.2337840002687507E-2</v>
+        <v>5.2333385428153696E-2</v>
       </c>
       <c r="G20" s="8">
         <f>A20-C20</f>
@@ -4982,7 +4985,7 @@
       </c>
       <c r="H20" s="8">
         <f t="shared" si="3"/>
-        <v>5.8375062184837514</v>
+        <v>5.8370093770676652</v>
       </c>
       <c r="I20" s="7">
         <v>0.99299999999999999</v>
@@ -5002,16 +5005,15 @@
         <v>82.219899999999996</v>
       </c>
       <c r="D21" s="6">
-        <f>29789431157/10000000</f>
-        <v>2978.9431156999999</v>
+        <v>2979</v>
       </c>
       <c r="E21" s="8">
         <f t="shared" si="1"/>
-        <v>2.9789431156999999</v>
+        <v>2.9790000000000001</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>3.6231412537597346E-2</v>
+        <v>3.6232104393218674E-2</v>
       </c>
       <c r="G21" s="8">
         <f t="shared" si="2"/>
@@ -5019,7 +5021,7 @@
       </c>
       <c r="H21" s="8">
         <f t="shared" si="3"/>
-        <v>4.2673393918194691</v>
+        <v>4.2674208786437351</v>
       </c>
       <c r="I21" s="7">
         <v>1</v>
@@ -5038,16 +5040,15 @@
         <v>99.901200000000003</v>
       </c>
       <c r="D22" s="6">
-        <f>38972066773/10000000</f>
-        <v>3897.2066773000001</v>
+        <v>3897</v>
       </c>
       <c r="E22" s="8">
         <f t="shared" si="1"/>
-        <v>3.8972066773000003</v>
+        <v>3.8969999999999998</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" ref="F22:F23" si="5">E22/C22</f>
-        <v>3.9010609254943887E-2</v>
+        <v>3.9008540437952696E-2</v>
       </c>
       <c r="G22" s="8">
         <f>A22-C22</f>
@@ -5055,7 +5056,7 @@
       </c>
       <c r="H22" s="8">
         <f t="shared" ref="H22:H23" si="6">F22*G22</f>
-        <v>4.880180405062374</v>
+        <v>4.8799215985393563</v>
       </c>
       <c r="I22" s="7">
         <v>1</v>
@@ -5074,16 +5075,15 @@
         <v>118.018</v>
       </c>
       <c r="D23" s="6">
-        <f>50119697364/10000000</f>
-        <v>5011.9697364000003</v>
+        <v>5012</v>
       </c>
       <c r="E23" s="8">
         <f t="shared" si="1"/>
-        <v>5.0119697364000002</v>
+        <v>5.0119999999999996</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="5"/>
-        <v>4.2467841654662851E-2</v>
+        <v>4.2468098086732527E-2</v>
       </c>
       <c r="G23" s="8">
         <f t="shared" ref="G23" si="7">A23-C23</f>
@@ -5091,7 +5091,7 @@
       </c>
       <c r="H23" s="8">
         <f t="shared" si="6"/>
-        <v>5.6049906772657128</v>
+        <v>5.6050245216831325</v>
       </c>
       <c r="I23" s="7">
         <v>1</v>

</xml_diff>